<commit_message>
yin zhuo jiao yu time schedule
</commit_message>
<xml_diff>
--- a/程序员客栈项目/因卓科技教育平台/需求梳理final/因卓教育项目计划.xlsx
+++ b/程序员客栈项目/因卓科技教育平台/需求梳理final/因卓教育项目计划.xlsx
@@ -106,10 +106,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -203,22 +202,22 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>42850</c:v>
+                  <c:v>42853</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42887</c:v>
+                  <c:v>42906</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42931</c:v>
+                  <c:v>43003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42931</c:v>
+                  <c:v>43003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42931</c:v>
+                  <c:v>43003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>42887</c:v>
+                  <c:v>42906</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -245,7 +244,9 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -286,22 +287,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>30.052500000000002</c:v>
+                  <c:v>43.627499999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40.6875</c:v>
+                  <c:v>62.265000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>97.32</c:v>
+                  <c:v>93.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>97.32</c:v>
+                  <c:v>93.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>97.32</c:v>
+                  <c:v>87.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>142.94999999999999</c:v>
+                  <c:v>120.57</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -356,10 +357,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -380,7 +378,7 @@
         <c:axId val="375131712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="42850"/>
+          <c:min val="42853"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="t"/>
@@ -416,10 +414,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1065,10 +1060,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>560244</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>47699</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>585107</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>47211</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1364,7 +1359,7 @@
   <dimension ref="A2:E8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1398,17 +1393,18 @@
         <v>4</v>
       </c>
       <c r="B3" s="1">
-        <v>42850</v>
+        <v>42853</v>
       </c>
       <c r="C3">
-        <v>20.035</v>
+        <f>20.035+9.05</f>
+        <v>29.085000000000001</v>
       </c>
       <c r="D3">
         <f>C3 * 1.5</f>
-        <v>30.052500000000002</v>
+        <v>43.627499999999998</v>
       </c>
       <c r="E3" s="1">
-        <v>42880</v>
+        <v>42902</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1416,17 +1412,18 @@
         <v>5</v>
       </c>
       <c r="B4" s="1">
-        <v>42887</v>
+        <v>42906</v>
       </c>
       <c r="C4">
-        <v>27.125</v>
+        <f>22.63 + 18.88</f>
+        <v>41.51</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:D8" si="0">C4 * 1.5</f>
-        <v>40.6875</v>
+        <v>62.265000000000001</v>
       </c>
       <c r="E4" s="1">
-        <v>42927</v>
+        <v>43000</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1434,17 +1431,17 @@
         <v>7</v>
       </c>
       <c r="B5" s="1">
-        <v>42931</v>
+        <v>43003</v>
       </c>
       <c r="C5">
-        <v>64.88</v>
+        <v>62.5</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>97.32</v>
+        <v>93.75</v>
       </c>
       <c r="E5" s="1">
-        <v>43031</v>
+        <v>43065</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -1452,17 +1449,17 @@
         <v>8</v>
       </c>
       <c r="B6" s="1">
-        <v>42931</v>
+        <v>43003</v>
       </c>
       <c r="C6">
-        <v>64.88</v>
+        <v>62.5</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>97.32</v>
+        <v>93.75</v>
       </c>
       <c r="E6" s="1">
-        <v>43031</v>
+        <v>43065</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1470,17 +1467,17 @@
         <v>9</v>
       </c>
       <c r="B7" s="1">
-        <v>42931</v>
+        <v>43003</v>
       </c>
       <c r="C7">
-        <v>64.88</v>
+        <v>58.5</v>
       </c>
       <c r="D7">
         <f>C7 * 1.5</f>
-        <v>97.32</v>
+        <v>87.75</v>
       </c>
       <c r="E7" s="1">
-        <v>43031</v>
+        <v>43063</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1488,17 +1485,17 @@
         <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>42887</v>
+        <v>42906</v>
       </c>
       <c r="C8">
-        <f>88.3 +1 + 1 + 2 + 2 +1</f>
-        <v>95.3</v>
+        <f>80.38</f>
+        <v>80.38</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>142.94999999999999</v>
-      </c>
-      <c r="E8" s="2">
+        <v>120.57</v>
+      </c>
+      <c r="E8" s="1">
         <v>43031</v>
       </c>
     </row>
@@ -1512,8 +1509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Q32" sqref="Q32"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="W22" sqref="W22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>